<commit_message>
Prior to code optimisation
</commit_message>
<xml_diff>
--- a/metaDataDict.xlsx
+++ b/metaDataDict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billi\Dropbox\_PhD\Application Documents\CASA RA\RA OS NARRATE CASA\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B0FEE3-5433-4FDD-9C8A-F9596565E3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0D7840-F85F-4765-90A0-521D0889E608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18120" yWindow="-2575" windowWidth="14400" windowHeight="7290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19230" yWindow="-2750" windowWidth="14340" windowHeight="7260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="certificates" sheetId="2" r:id="rId1"/>
@@ -1410,18 +1410,18 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="30.2265625" customWidth="1"/>
-    <col min="3" max="3" width="3.26953125" customWidth="1"/>
+    <col min="2" max="2" width="36.04296875" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
     <col min="4" max="4" width="15.453125" customWidth="1"/>
-    <col min="5" max="5" width="4.26953125" customWidth="1"/>
-    <col min="6" max="6" width="2.58984375" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" customWidth="1"/>
+    <col min="6" max="6" width="6.2265625" customWidth="1"/>
     <col min="7" max="7" width="11.453125" customWidth="1"/>
     <col min="8" max="8" width="10.6328125" customWidth="1"/>
   </cols>
@@ -1452,7 +1452,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>10001893276</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
+    <row r="87" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:8" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2674,9 +2674,9 @@
   </sheetData>
   <autoFilter ref="A1:G93" xr:uid="{DE7C778E-0956-4964-9956-6AE5B0E9DAA8}">
     <filterColumn colId="4">
-      <filters>
-        <filter val="?"/>
-      </filters>
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>